<commit_message>
updated SSM flight BOM in compiled flight BOM excel, [SSM] minor BOM update
</commit_message>
<xml_diff>
--- a/payload/pay-ssm/Project Outputs for pay-ssm/pay-ssm-BOM.xlsx
+++ b/payload/pay-ssm/Project Outputs for pay-ssm/pay-ssm-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorna\pcbs\payload\pay-ssm\Project Outputs for pay-ssm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8DDBCD73-B6F7-4A68-97F4-F26CF96FC1A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFB6DE13-7478-4CBB-84E0-FDA93DF986DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{D80D1A47-8443-45DF-AB6C-FA8382952EC4}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{36C01730-AC10-428D-8BEB-B64C290D3C6E}"/>
   </bookViews>
   <sheets>
     <sheet name="pay-ssm-BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="257">
   <si>
     <t>Line #</t>
   </si>
@@ -168,13 +168,13 @@
     <t>490-3261-1-ND</t>
   </si>
   <si>
-    <t>C36_MOTOR_DRV1, C36_MOTOR_DRV2</t>
-  </si>
-  <si>
-    <t>10000pF 25V</t>
-  </si>
-  <si>
-    <t>445-6900-1-ND</t>
+    <t>C36_MOTOR_DRV1, C36_MOTOR_DRV2, C53</t>
+  </si>
+  <si>
+    <t>10000pF</t>
+  </si>
+  <si>
+    <t>490-4762-1-ND</t>
   </si>
   <si>
     <t>C42, C44</t>
@@ -213,16 +213,7 @@
     <t>490-5869-1-ND</t>
   </si>
   <si>
-    <t>C53</t>
-  </si>
-  <si>
-    <t>10000pF</t>
-  </si>
-  <si>
-    <t>490-4762-1-ND</t>
-  </si>
-  <si>
-    <t>R1, R2, R17, R18, R69_Port_Expander1, R69_Port_Expander2, R70_Port_Expander1, R70_Port_Expander2, R71_Port_Expander1, R71_Port_Expander2, R72_Port_Expander1, R72_Port_Expander2, R73_Port_Expander1, R73_Port_Expander2, R74_Port_Expander1, R74_Port_Expander2</t>
+    <t>R1, R2, R17, R18, R27, R31, R40, R69_Port_Expander1, R69_Port_Expander2, R70_Port_Expander1, R70_Port_Expander2, R71_Port_Expander1, R71_Port_Expander2, R72_Port_Expander1, R72_Port_Expander2, R73_Port_Expander1, R73_Port_Expander2, R74_Port_Expander1, R74_Port_Expander2, R90</t>
   </si>
   <si>
     <t>P0.0JCT-ND</t>
@@ -256,15 +247,6 @@
   </si>
   <si>
     <t>P10.0KLCT-ND</t>
-  </si>
-  <si>
-    <t>R27, R31, R40, R90</t>
-  </si>
-  <si>
-    <t>0ohm</t>
-  </si>
-  <si>
-    <t>RMCF0402ZT0R00CT-ND</t>
   </si>
   <si>
     <t>R30</t>
@@ -1193,11 +1175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFD96307-2708-4694-BEC2-F89ACDC1EE5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F6C9AD-2928-436D-9BD1-FF3C4E8180C9}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1205,7 +1187,7 @@
   <cols>
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" customWidth="1"/>
+    <col min="3" max="3" width="54.6640625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="13.109375" customWidth="1"/>
@@ -1264,10 +1246,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="1">
-        <v>0.19872999999999999</v>
+        <v>0.1991</v>
       </c>
       <c r="I2" s="1">
-        <v>0.19872999999999999</v>
+        <v>0.1991</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1316,10 +1298,10 @@
         <v>19</v>
       </c>
       <c r="H4" s="1">
-        <v>0.17554</v>
+        <v>0.17619000000000001</v>
       </c>
       <c r="I4" s="1">
-        <v>0.87768000000000002</v>
+        <v>0.88092999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1343,10 +1325,10 @@
         <v>22</v>
       </c>
       <c r="H5" s="1">
-        <v>0.25173000000000001</v>
+        <v>0.25219999999999998</v>
       </c>
       <c r="I5" s="1">
-        <v>0.50346000000000002</v>
+        <v>0.50439000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1368,10 +1350,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="1">
-        <v>9.128E-2</v>
+        <v>9.1619999999999993E-2</v>
       </c>
       <c r="I6" s="1">
-        <v>0.91278999999999999</v>
+        <v>0.91617000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1395,10 +1377,10 @@
         <v>26</v>
       </c>
       <c r="H7" s="1">
-        <v>0.17224</v>
+        <v>0.17255999999999999</v>
       </c>
       <c r="I7" s="1">
-        <v>0.17224</v>
+        <v>0.17255999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1422,10 +1404,10 @@
         <v>29</v>
       </c>
       <c r="H8" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I8" s="1">
-        <v>0.26497999999999999</v>
+        <v>0.26546999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1449,10 +1431,10 @@
         <v>32</v>
       </c>
       <c r="H9" s="1">
-        <v>4.505E-2</v>
+        <v>4.5130000000000003E-2</v>
       </c>
       <c r="I9" s="1">
-        <v>0.45046999999999998</v>
+        <v>0.45129999999999998</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1476,10 +1458,10 @@
         <v>35</v>
       </c>
       <c r="H10" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I10" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1503,10 +1485,10 @@
         <v>38</v>
       </c>
       <c r="H11" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>0.26497999999999999</v>
+        <v>0.26546999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1530,10 +1512,10 @@
         <v>41</v>
       </c>
       <c r="H12" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I12" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1557,10 +1539,10 @@
         <v>44</v>
       </c>
       <c r="H13" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I13" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1575,7 +1557,7 @@
         <v>46</v>
       </c>
       <c r="E14" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>12</v>
@@ -1584,10 +1566,10 @@
         <v>47</v>
       </c>
       <c r="H14" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I14" s="1">
-        <v>0.26497999999999999</v>
+        <v>0.3982</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1611,10 +1593,10 @@
         <v>50</v>
       </c>
       <c r="H15" s="1">
-        <v>0.14574000000000001</v>
+        <v>0.14601</v>
       </c>
       <c r="I15" s="1">
-        <v>0.29148000000000002</v>
+        <v>0.29202</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1638,10 +1620,10 @@
         <v>53</v>
       </c>
       <c r="H16" s="1">
-        <v>0.14574000000000001</v>
+        <v>0.14601</v>
       </c>
       <c r="I16" s="1">
-        <v>0.14574000000000001</v>
+        <v>0.14601</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1665,10 +1647,10 @@
         <v>56</v>
       </c>
       <c r="H17" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I17" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1692,10 +1674,10 @@
         <v>59</v>
       </c>
       <c r="H18" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I18" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1706,23 +1688,23 @@
       <c r="C19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>20</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="H19" s="1">
-        <v>0.13249</v>
+        <v>2.8670000000000001E-2</v>
       </c>
       <c r="I19" s="1">
-        <v>0.13249</v>
+        <v>0.71677000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1731,25 +1713,25 @@
         <v>402</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="1">
+        <v>100</v>
+      </c>
+      <c r="E20" s="1">
+        <v>19</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>16</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="H20" s="1">
-        <v>3.9750000000000001E-2</v>
+        <v>0.18317</v>
       </c>
       <c r="I20" s="1">
-        <v>0.63595000000000002</v>
+        <v>3.48</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1758,13 +1740,13 @@
         <v>402</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="1">
-        <v>100</v>
-      </c>
       <c r="E21" s="1">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>12</v>
@@ -1773,10 +1755,10 @@
         <v>66</v>
       </c>
       <c r="H21" s="1">
-        <v>0.18284</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I21" s="1">
-        <v>3.47</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1787,23 +1769,23 @@
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" s="1">
+        <v>60.4</v>
+      </c>
+      <c r="E22" s="1">
+        <v>2</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="H22" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I22" s="1">
-        <v>0.13249</v>
+        <v>0.26546999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1812,13 +1794,13 @@
         <v>402</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D23" s="1">
-        <v>60.4</v>
-      </c>
       <c r="E23" s="1">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>12</v>
@@ -1827,10 +1809,10 @@
         <v>71</v>
       </c>
       <c r="H23" s="1">
-        <v>0.13249</v>
+        <v>5.9729999999999998E-2</v>
       </c>
       <c r="I23" s="1">
-        <v>0.26497999999999999</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1845,7 +1827,7 @@
         <v>73</v>
       </c>
       <c r="E24" s="1">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>12</v>
@@ -1854,10 +1836,10 @@
         <v>74</v>
       </c>
       <c r="H24" s="1">
-        <v>5.9619999999999999E-2</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I24" s="1">
-        <v>2.0299999999999998</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1872,7 +1854,7 @@
         <v>76</v>
       </c>
       <c r="E25" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>12</v>
@@ -1881,10 +1863,10 @@
         <v>77</v>
       </c>
       <c r="H25" s="1">
-        <v>1.5900000000000001E-2</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I25" s="1">
-        <v>0.15898999999999999</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1908,10 +1890,10 @@
         <v>80</v>
       </c>
       <c r="H26" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I26" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1926,7 +1908,7 @@
         <v>82</v>
       </c>
       <c r="E27" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
@@ -1935,10 +1917,10 @@
         <v>83</v>
       </c>
       <c r="H27" s="1">
-        <v>0.13249</v>
+        <v>1.7260000000000001E-2</v>
       </c>
       <c r="I27" s="1">
-        <v>0.13249</v>
+        <v>0.25883</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1953,7 +1935,7 @@
         <v>85</v>
       </c>
       <c r="E28" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>12</v>
@@ -1962,10 +1944,10 @@
         <v>86</v>
       </c>
       <c r="H28" s="1">
-        <v>0.13249</v>
+        <v>0.1991</v>
       </c>
       <c r="I28" s="1">
-        <v>0.13249</v>
+        <v>0.99551000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1980,7 +1962,7 @@
         <v>88</v>
       </c>
       <c r="E29" s="1">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>12</v>
@@ -1989,10 +1971,10 @@
         <v>89</v>
       </c>
       <c r="H29" s="1">
-        <v>1.7219999999999999E-2</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I29" s="1">
-        <v>0.25835999999999998</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -2007,7 +1989,7 @@
         <v>91</v>
       </c>
       <c r="E30" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
@@ -2016,10 +1998,10 @@
         <v>92</v>
       </c>
       <c r="H30" s="1">
-        <v>0.19872999999999999</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I30" s="1">
-        <v>0.99367000000000005</v>
+        <v>0.26546999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2034,7 +2016,7 @@
         <v>94</v>
       </c>
       <c r="E31" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>12</v>
@@ -2043,10 +2025,10 @@
         <v>95</v>
       </c>
       <c r="H31" s="1">
-        <v>0.13249</v>
+        <v>5.9729999999999998E-2</v>
       </c>
       <c r="I31" s="1">
-        <v>0.13249</v>
+        <v>0.59731000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -2057,23 +2039,23 @@
       <c r="C32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="D32" s="1">
+        <v>330</v>
+      </c>
+      <c r="E32" s="1">
+        <v>8</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E32" s="1">
-        <v>2</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="H32" s="1">
-        <v>0.13249</v>
+        <v>2.92E-2</v>
       </c>
       <c r="I32" s="1">
-        <v>0.26497999999999999</v>
+        <v>0.29202</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2082,25 +2064,25 @@
         <v>402</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E33" s="1">
-        <v>6</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="H33" s="1">
-        <v>5.9619999999999999E-2</v>
+        <v>0.42608000000000001</v>
       </c>
       <c r="I33" s="1">
-        <v>0.59619999999999995</v>
+        <v>7.24</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -2109,13 +2091,13 @@
         <v>402</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D34" s="1">
-        <v>330</v>
-      </c>
       <c r="E34" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>12</v>
@@ -2124,10 +2106,10 @@
         <v>103</v>
       </c>
       <c r="H34" s="1">
-        <v>2.9149999999999999E-2</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I34" s="1">
-        <v>0.29148000000000002</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2142,7 +2124,7 @@
         <v>105</v>
       </c>
       <c r="E35" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>12</v>
@@ -2151,10 +2133,10 @@
         <v>106</v>
       </c>
       <c r="H35" s="1">
-        <v>0.42529</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I35" s="1">
-        <v>7.23</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2178,10 +2160,10 @@
         <v>109</v>
       </c>
       <c r="H36" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I36" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
@@ -2205,10 +2187,10 @@
         <v>112</v>
       </c>
       <c r="H37" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I37" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
@@ -2219,23 +2201,23 @@
       <c r="C38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D38" s="1">
+        <v>2</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>115</v>
-      </c>
       <c r="H38" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I38" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
@@ -2244,40 +2226,40 @@
         <v>402</v>
       </c>
       <c r="C39" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="D39" s="1" t="s">
+      <c r="E39" s="1">
+        <v>1</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="1">
-        <v>1</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="1" t="s">
-        <v>118</v>
-      </c>
       <c r="H39" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I39" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="D40" s="1">
-        <v>2</v>
-      </c>
       <c r="E40" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>12</v>
@@ -2286,16 +2268,16 @@
         <v>120</v>
       </c>
       <c r="H40" s="1">
-        <v>0.13249</v>
+        <v>0.14468</v>
       </c>
       <c r="I40" s="1">
-        <v>0.13249</v>
+        <v>1.45</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>121</v>
@@ -2313,10 +2295,10 @@
         <v>123</v>
       </c>
       <c r="H41" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I41" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -2331,7 +2313,7 @@
         <v>125</v>
       </c>
       <c r="E42" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>12</v>
@@ -2340,10 +2322,10 @@
         <v>126</v>
       </c>
       <c r="H42" s="1">
-        <v>0.14441000000000001</v>
+        <v>0.35837999999999998</v>
       </c>
       <c r="I42" s="1">
-        <v>1.44</v>
+        <v>0.71677000000000002</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2355,7 +2337,7 @@
         <v>127</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="E43" s="1">
         <v>1</v>
@@ -2364,13 +2346,13 @@
         <v>12</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="H43" s="1">
-        <v>0.13249</v>
+        <v>0.1991</v>
       </c>
       <c r="I43" s="1">
-        <v>0.13249</v>
+        <v>0.1991</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2379,25 +2361,25 @@
         <v>603</v>
       </c>
       <c r="C44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="E44" s="1">
-        <v>2</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="H44" s="1">
-        <v>0.35771999999999998</v>
+        <v>0.29202</v>
       </c>
       <c r="I44" s="1">
-        <v>0.71545000000000003</v>
+        <v>0.29202</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
@@ -2406,25 +2388,25 @@
         <v>603</v>
       </c>
       <c r="C45" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="1">
+        <v>6</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E45" s="1">
-        <v>1</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="H45" s="1">
-        <v>0.19872999999999999</v>
+        <v>0.82296000000000002</v>
       </c>
       <c r="I45" s="1">
-        <v>0.19872999999999999</v>
+        <v>4.9400000000000004</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
@@ -2448,10 +2430,10 @@
         <v>136</v>
       </c>
       <c r="H46" s="1">
-        <v>0.29148000000000002</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I46" s="1">
-        <v>0.29148000000000002</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
@@ -2466,7 +2448,7 @@
         <v>138</v>
       </c>
       <c r="E47" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>12</v>
@@ -2475,16 +2457,16 @@
         <v>139</v>
       </c>
       <c r="H47" s="1">
-        <v>0.82143999999999995</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I47" s="1">
-        <v>4.93</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="1">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>140</v>
@@ -2493,7 +2475,7 @@
         <v>141</v>
       </c>
       <c r="E48" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>12</v>
@@ -2502,16 +2484,16 @@
         <v>142</v>
       </c>
       <c r="H48" s="1">
-        <v>0.13249</v>
+        <v>0.51093999999999995</v>
       </c>
       <c r="I48" s="1">
-        <v>0.13249</v>
+        <v>5.1100000000000003</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1"/>
       <c r="B49" s="1">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>143</v>
@@ -2520,19 +2502,19 @@
         <v>144</v>
       </c>
       <c r="E49" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="H49" s="1">
-        <v>0.13249</v>
+        <v>0.73997999999999997</v>
       </c>
       <c r="I49" s="1">
-        <v>0.13249</v>
+        <v>1.48</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2541,25 +2523,25 @@
         <v>805</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E50" s="1">
-        <v>8</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="H50" s="1">
-        <v>0.50905</v>
+        <v>0.42475000000000002</v>
       </c>
       <c r="I50" s="1">
-        <v>5.09</v>
+        <v>0.84950000000000003</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2568,10 +2550,10 @@
         <v>805</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -2580,13 +2562,13 @@
         <v>12</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H51" s="1">
-        <v>0.73724999999999996</v>
+        <v>0.83623000000000003</v>
       </c>
       <c r="I51" s="1">
-        <v>1.47</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2598,22 +2580,22 @@
         <v>151</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E52" s="1">
-        <v>2</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>153</v>
-      </c>
       <c r="H52" s="1">
-        <v>0.42397000000000001</v>
+        <v>0.55749000000000004</v>
       </c>
       <c r="I52" s="1">
-        <v>0.84794000000000003</v>
+        <v>0.55749000000000004</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -2622,25 +2604,25 @@
         <v>805</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="D53" s="1" t="s">
+      <c r="E53" s="1">
+        <v>1</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E53" s="1">
-        <v>2</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="H53" s="1">
-        <v>0.83469000000000004</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I53" s="1">
-        <v>1.67</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -2649,13 +2631,13 @@
         <v>805</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="1" t="s">
-        <v>147</v>
-      </c>
       <c r="E54" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F54" s="1" t="s">
         <v>12</v>
@@ -2664,10 +2646,10 @@
         <v>158</v>
       </c>
       <c r="H54" s="1">
-        <v>0.55645999999999995</v>
+        <v>0.86277999999999999</v>
       </c>
       <c r="I54" s="1">
-        <v>0.55645999999999995</v>
+        <v>1.73</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
@@ -2691,10 +2673,10 @@
         <v>161</v>
       </c>
       <c r="H55" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
       <c r="I55" s="1">
-        <v>0.13249</v>
+        <v>0.13272999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
@@ -2709,7 +2691,7 @@
         <v>163</v>
       </c>
       <c r="E56" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>12</v>
@@ -2718,16 +2700,16 @@
         <v>164</v>
       </c>
       <c r="H56" s="1">
-        <v>0.86117999999999995</v>
+        <v>1.04</v>
       </c>
       <c r="I56" s="1">
-        <v>1.72</v>
+        <v>8.2799999999999994</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
       <c r="B57" s="1">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>165</v>
@@ -2736,7 +2718,7 @@
         <v>166</v>
       </c>
       <c r="E57" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>12</v>
@@ -2745,16 +2727,16 @@
         <v>167</v>
       </c>
       <c r="H57" s="1">
-        <v>0.13249</v>
+        <v>1.29</v>
       </c>
       <c r="I57" s="1">
-        <v>0.13249</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
       <c r="B58" s="1">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>168</v>
@@ -2763,7 +2745,7 @@
         <v>169</v>
       </c>
       <c r="E58" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -2772,10 +2754,10 @@
         <v>170</v>
       </c>
       <c r="H58" s="1">
-        <v>1.03</v>
+        <v>1.59</v>
       </c>
       <c r="I58" s="1">
-        <v>8.27</v>
+        <v>3.19</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
@@ -2790,7 +2772,7 @@
         <v>172</v>
       </c>
       <c r="E59" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -2799,16 +2781,16 @@
         <v>173</v>
       </c>
       <c r="H59" s="1">
-        <v>1.29</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I59" s="1">
-        <v>2.57</v>
+        <v>6.85</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
       <c r="B60" s="1">
-        <v>1206</v>
+        <v>2220</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>174</v>
@@ -2817,7 +2799,7 @@
         <v>175</v>
       </c>
       <c r="E60" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>12</v>
@@ -2826,25 +2808,23 @@
         <v>176</v>
       </c>
       <c r="H60" s="1">
-        <v>1.59</v>
+        <v>3.42</v>
       </c>
       <c r="I60" s="1">
-        <v>3.18</v>
+        <v>10.27</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
-      <c r="B61" s="1">
-        <v>1206</v>
+      <c r="B61" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="D61" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="D61" s="1"/>
       <c r="E61" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>12</v>
@@ -2853,25 +2833,23 @@
         <v>179</v>
       </c>
       <c r="H61" s="1">
-        <v>1.1399999999999999</v>
+        <v>1.82</v>
       </c>
       <c r="I61" s="1">
-        <v>6.84</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
-      <c r="B62" s="1">
-        <v>2220</v>
+      <c r="B62" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D62" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="D62" s="1"/>
       <c r="E62" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>12</v>
@@ -2880,10 +2858,10 @@
         <v>182</v>
       </c>
       <c r="H62" s="1">
-        <v>3.42</v>
+        <v>12.19</v>
       </c>
       <c r="I62" s="1">
-        <v>10.25</v>
+        <v>24.37</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
@@ -2896,7 +2874,7 @@
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F63" s="1" t="s">
         <v>12</v>
@@ -2905,10 +2883,10 @@
         <v>185</v>
       </c>
       <c r="H63" s="1">
-        <v>1.82</v>
+        <v>7.13</v>
       </c>
       <c r="I63" s="1">
-        <v>3.63</v>
+        <v>7.13</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
@@ -2921,7 +2899,7 @@
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>12</v>
@@ -2930,10 +2908,10 @@
         <v>188</v>
       </c>
       <c r="H64" s="1">
-        <v>12.16</v>
+        <v>0.57076000000000005</v>
       </c>
       <c r="I64" s="1">
-        <v>24.33</v>
+        <v>5.14</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
@@ -2946,7 +2924,7 @@
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>12</v>
@@ -2955,10 +2933,10 @@
         <v>191</v>
       </c>
       <c r="H65" s="1">
-        <v>7.11</v>
+        <v>1.31</v>
       </c>
       <c r="I65" s="1">
-        <v>7.11</v>
+        <v>2.63</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
@@ -2971,7 +2949,7 @@
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>12</v>
@@ -2980,10 +2958,10 @@
         <v>194</v>
       </c>
       <c r="H66" s="1">
-        <v>0.56971000000000005</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="I66" s="1">
-        <v>5.13</v>
+        <v>4.49</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
@@ -2996,7 +2974,7 @@
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>12</v>
@@ -3005,10 +2983,10 @@
         <v>197</v>
       </c>
       <c r="H67" s="1">
-        <v>1.31</v>
+        <v>1.61</v>
       </c>
       <c r="I67" s="1">
-        <v>2.62</v>
+        <v>1.61</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
@@ -3030,10 +3008,10 @@
         <v>200</v>
       </c>
       <c r="H68" s="1">
-        <v>2.2400000000000002</v>
+        <v>3.66</v>
       </c>
       <c r="I68" s="1">
-        <v>4.4800000000000004</v>
+        <v>7.33</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
@@ -3055,10 +3033,10 @@
         <v>203</v>
       </c>
       <c r="H69" s="1">
-        <v>1.6</v>
+        <v>16.41</v>
       </c>
       <c r="I69" s="1">
-        <v>1.6</v>
+        <v>16.41</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
@@ -3071,7 +3049,7 @@
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>12</v>
@@ -3080,10 +3058,10 @@
         <v>206</v>
       </c>
       <c r="H70" s="1">
-        <v>3.66</v>
+        <v>1.92</v>
       </c>
       <c r="I70" s="1">
-        <v>7.31</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
@@ -3096,7 +3074,7 @@
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>12</v>
@@ -3105,10 +3083,10 @@
         <v>209</v>
       </c>
       <c r="H71" s="1">
-        <v>16.38</v>
+        <v>2.27</v>
       </c>
       <c r="I71" s="1">
-        <v>16.38</v>
+        <v>4.54</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
@@ -3121,7 +3099,7 @@
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>12</v>
@@ -3130,10 +3108,10 @@
         <v>212</v>
       </c>
       <c r="H72" s="1">
-        <v>1.92</v>
+        <v>0.40350999999999998</v>
       </c>
       <c r="I72" s="1">
-        <v>1.92</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
@@ -3155,10 +3133,10 @@
         <v>215</v>
       </c>
       <c r="H73" s="1">
-        <v>2.27</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="I73" s="1">
-        <v>4.53</v>
+        <v>4.1399999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
@@ -3171,7 +3149,7 @@
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>12</v>
@@ -3180,10 +3158,10 @@
         <v>218</v>
       </c>
       <c r="H74" s="1">
-        <v>0.40277000000000002</v>
+        <v>0.40616999999999998</v>
       </c>
       <c r="I74" s="1">
-        <v>5.24</v>
+        <v>4.0599999999999996</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
@@ -3205,10 +3183,10 @@
         <v>221</v>
       </c>
       <c r="H75" s="1">
-        <v>2.0699999999999998</v>
+        <v>3.98</v>
       </c>
       <c r="I75" s="1">
-        <v>4.13</v>
+        <v>7.96</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -3221,7 +3199,7 @@
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>12</v>
@@ -3230,10 +3208,10 @@
         <v>224</v>
       </c>
       <c r="H76" s="1">
-        <v>0.40542</v>
+        <v>5.35</v>
       </c>
       <c r="I76" s="1">
-        <v>4.05</v>
+        <v>5.35</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
@@ -3246,7 +3224,7 @@
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>12</v>
@@ -3255,10 +3233,10 @@
         <v>227</v>
       </c>
       <c r="H77" s="1">
-        <v>3.97</v>
+        <v>1.02</v>
       </c>
       <c r="I77" s="1">
-        <v>7.95</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
@@ -3280,10 +3258,10 @@
         <v>230</v>
       </c>
       <c r="H78" s="1">
-        <v>5.34</v>
+        <v>3.03</v>
       </c>
       <c r="I78" s="1">
-        <v>5.34</v>
+        <v>3.03</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
@@ -3305,10 +3283,10 @@
         <v>233</v>
       </c>
       <c r="H79" s="1">
-        <v>1.02</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I79" s="1">
-        <v>1.02</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
@@ -3330,10 +3308,10 @@
         <v>236</v>
       </c>
       <c r="H80" s="1">
-        <v>3.02</v>
+        <v>0.88932</v>
       </c>
       <c r="I80" s="1">
-        <v>3.02</v>
+        <v>0.88932</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
@@ -3355,10 +3333,10 @@
         <v>239</v>
       </c>
       <c r="H81" s="1">
-        <v>4.1500000000000004</v>
+        <v>0.67695000000000005</v>
       </c>
       <c r="I81" s="1">
-        <v>4.1500000000000004</v>
+        <v>0.67695000000000005</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
@@ -3371,7 +3349,7 @@
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>12</v>
@@ -3380,10 +3358,10 @@
         <v>242</v>
       </c>
       <c r="H82" s="1">
-        <v>0.88768000000000002</v>
+        <v>5.87</v>
       </c>
       <c r="I82" s="1">
-        <v>0.88768000000000002</v>
+        <v>11.73</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
@@ -3399,66 +3377,66 @@
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>12</v>
+        <v>245</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H83" s="1">
-        <v>0.67569999999999997</v>
+        <v>0.59731000000000001</v>
       </c>
       <c r="I83" s="1">
-        <v>0.67569999999999997</v>
+        <v>0.59731000000000001</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1"/>
       <c r="B84" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>12</v>
+        <v>245</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="H84" s="1">
-        <v>5.86</v>
+        <v>28.96</v>
       </c>
       <c r="I84" s="1">
-        <v>11.71</v>
+        <v>28.96</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1"/>
       <c r="B85" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1">
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G85" s="1" t="s">
         <v>252</v>
       </c>
       <c r="H85" s="1">
-        <v>0.59619999999999995</v>
+        <v>1.62</v>
       </c>
       <c r="I85" s="1">
-        <v>0.59619999999999995</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
@@ -3469,78 +3447,28 @@
       <c r="C86" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="D86" s="1"/>
+      <c r="D86" s="1" t="s">
+        <v>255</v>
+      </c>
       <c r="E86" s="1">
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="H86" s="1">
-        <v>28.91</v>
+        <v>2.81</v>
       </c>
       <c r="I86" s="1">
-        <v>28.91</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>257</v>
-      </c>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1">
-        <v>1</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="H87" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="I87" s="1">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1" t="s">
-        <v>259</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="E88" s="1">
-        <v>1</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="H88" s="1">
-        <v>2.81</v>
-      </c>
-      <c r="I88" s="1">
         <v>2.81</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="38" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="39" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[SSM] final BOM update
</commit_message>
<xml_diff>
--- a/payload/pay-ssm/Project Outputs for pay-ssm/pay-ssm-BOM.xlsx
+++ b/payload/pay-ssm/Project Outputs for pay-ssm/pay-ssm-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorna\pcbs\payload\pay-ssm\Project Outputs for pay-ssm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lorna.l\pcbs\payload\pay-ssm\Project Outputs for pay-ssm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFB6DE13-7478-4CBB-84E0-FDA93DF986DD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE75C9A3-4F84-49FC-BBC0-E5305200AD16}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9420" xr2:uid="{36C01730-AC10-428D-8BEB-B64C290D3C6E}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{B9BB9968-4510-4C9B-B638-FF600D63CD46}"/>
   </bookViews>
   <sheets>
     <sheet name="pay-ssm-BOM" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="247">
   <si>
     <t>Line #</t>
   </si>
@@ -84,7 +84,7 @@
     <t>535-13456-1-ND</t>
   </si>
   <si>
-    <t>C2, C3, C4, C46_Current_Monitor1, C46_Current_Monitor2</t>
+    <t>C2, C3, C4, C8, C10_ADC1, C10_ADC2, C45_Port_Expander1, C45_Port_Expander2, C46_Current_Monitor1, C46_Current_Monitor2, C56</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -102,9 +102,6 @@
     <t>399-17554-1-ND</t>
   </si>
   <si>
-    <t>C8, C10_ADC1, C10_ADC2, C45_Port_Expander1, C45_Port_Expander2, C56</t>
-  </si>
-  <si>
     <t>C9</t>
   </si>
   <si>
@@ -123,13 +120,10 @@
     <t>490-4912-1-ND</t>
   </si>
   <si>
-    <t>C20, C30, C32, C52</t>
-  </si>
-  <si>
-    <t>0.1uF 10V X7R</t>
-  </si>
-  <si>
-    <t>490-6321-1-ND</t>
+    <t>C20, C30, C31, C32, C42, C44, C52</t>
+  </si>
+  <si>
+    <t>0.1uF 16V X7R</t>
   </si>
   <si>
     <t>C26</t>
@@ -159,15 +153,6 @@
     <t>490-6178-1-ND</t>
   </si>
   <si>
-    <t>C31</t>
-  </si>
-  <si>
-    <t>0.1uF 16V X7R</t>
-  </si>
-  <si>
-    <t>490-3261-1-ND</t>
-  </si>
-  <si>
     <t>C36_MOTOR_DRV1, C36_MOTOR_DRV2, C53</t>
   </si>
   <si>
@@ -177,15 +162,6 @@
     <t>490-4762-1-ND</t>
   </si>
   <si>
-    <t>C42, C44</t>
-  </si>
-  <si>
-    <t>0.1uF 6.3V X7R</t>
-  </si>
-  <si>
-    <t>399-4872-1-ND</t>
-  </si>
-  <si>
     <t>C43</t>
   </si>
   <si>
@@ -291,7 +267,7 @@
     <t>10K NTC</t>
   </si>
   <si>
-    <t>P12007DKR-ND</t>
+    <t>P12007CT-ND</t>
   </si>
   <si>
     <t>R39</t>
@@ -453,7 +429,7 @@
     <t>311-470KHRCT-ND</t>
   </si>
   <si>
-    <t>C1, C7, C12_ADC1, C12_ADC2, C18_ADS79521, C18_ADS79522, C41_Port_Expander1, C41_Port_Expander2</t>
+    <t>C1, C7, C12_ADC1, C12_ADC2, C18_ADS79521, C18_ADS79522, C41_Port_Expander1, C41_Port_Expander2, C55</t>
   </si>
   <si>
     <t>10uF</t>
@@ -484,12 +460,6 @@
   </si>
   <si>
     <t>445-11470-1-ND</t>
-  </si>
-  <si>
-    <t>C55</t>
-  </si>
-  <si>
-    <t>490-14361-6-ND</t>
   </si>
   <si>
     <t>R26</t>
@@ -1175,11 +1145,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2F6C9AD-2928-436D-9BD1-FF3C4E8180C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B99B8F8-9B1F-41F4-AA80-84470E1C0551}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1188,7 +1158,7 @@
     <col min="1" max="1" width="10.33203125" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" customWidth="1"/>
     <col min="3" max="3" width="54.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="22.109375" customWidth="1"/>
@@ -1246,10 +1216,10 @@
         <v>13</v>
       </c>
       <c r="H2" s="1">
-        <v>0.1991</v>
+        <v>0.19869000000000001</v>
       </c>
       <c r="I2" s="1">
-        <v>0.1991</v>
+        <v>0.19869000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -1289,7 +1259,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="1">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>12</v>
@@ -1298,10 +1268,10 @@
         <v>19</v>
       </c>
       <c r="H4" s="1">
-        <v>0.17619000000000001</v>
+        <v>9.1240000000000002E-2</v>
       </c>
       <c r="I4" s="1">
-        <v>0.88092999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1325,10 +1295,10 @@
         <v>22</v>
       </c>
       <c r="H5" s="1">
-        <v>0.25219999999999998</v>
+        <v>0.25168000000000001</v>
       </c>
       <c r="I5" s="1">
-        <v>0.50439000000000001</v>
+        <v>0.50334999999999996</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1339,21 +1309,23 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="E6" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="H6" s="1">
-        <v>9.1619999999999993E-2</v>
+        <v>0.17219999999999999</v>
       </c>
       <c r="I6" s="1">
-        <v>0.91617000000000004</v>
+        <v>0.17219999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
@@ -1362,25 +1334,25 @@
         <v>402</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H7" s="1">
-        <v>0.17255999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I7" s="1">
-        <v>0.17255999999999999</v>
+        <v>0.26491999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -1389,25 +1361,25 @@
         <v>402</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E8" s="1">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="H8" s="1">
-        <v>0.13272999999999999</v>
+        <v>9.1240000000000002E-2</v>
       </c>
       <c r="I8" s="1">
-        <v>0.26546999999999998</v>
+        <v>0.91239000000000003</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1416,25 +1388,25 @@
         <v>402</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E9" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H9" s="1">
-        <v>4.5130000000000003E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I9" s="1">
-        <v>0.45129999999999998</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -1443,25 +1415,25 @@
         <v>402</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H10" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I10" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.26491999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -1470,25 +1442,25 @@
         <v>402</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H11" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I11" s="1">
-        <v>0.26546999999999998</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
@@ -1497,25 +1469,25 @@
         <v>402</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I12" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.39738000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -1524,10 +1496,10 @@
         <v>402</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
@@ -1536,13 +1508,13 @@
         <v>12</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H13" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.14571000000000001</v>
       </c>
       <c r="I13" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.14571000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -1551,25 +1523,25 @@
         <v>402</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E14" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H14" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I14" s="1">
-        <v>0.3982</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1578,25 +1550,25 @@
         <v>402</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E15" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H15" s="1">
-        <v>0.14601</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I15" s="1">
-        <v>0.29202</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -1605,13 +1577,13 @@
         <v>402</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D16" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
       <c r="E16" s="1">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>12</v>
@@ -1620,10 +1592,10 @@
         <v>53</v>
       </c>
       <c r="H16" s="1">
-        <v>0.14601</v>
+        <v>2.861E-2</v>
       </c>
       <c r="I16" s="1">
-        <v>0.14601</v>
+        <v>0.71528999999999998</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -1634,23 +1606,23 @@
       <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="1">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="H17" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.18279999999999999</v>
       </c>
       <c r="I17" s="1">
-        <v>0.13272999999999999</v>
+        <v>3.47</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1659,25 +1631,25 @@
         <v>402</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="H18" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I18" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1686,25 +1658,25 @@
         <v>402</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="1">
+        <v>60.4</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>20</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="H19" s="1">
-        <v>2.8670000000000001E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I19" s="1">
-        <v>0.71677000000000002</v>
+        <v>0.26491999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1713,13 +1685,13 @@
         <v>402</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="1">
-        <v>100</v>
-      </c>
       <c r="E20" s="1">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>12</v>
@@ -1728,10 +1700,10 @@
         <v>63</v>
       </c>
       <c r="H20" s="1">
-        <v>0.18317</v>
+        <v>5.9610000000000003E-2</v>
       </c>
       <c r="I20" s="1">
-        <v>3.48</v>
+        <v>2.0299999999999998</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1755,10 +1727,10 @@
         <v>66</v>
       </c>
       <c r="H21" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I21" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1769,23 +1741,23 @@
       <c r="C22" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="1">
-        <v>60.4</v>
+      <c r="D22" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="E22" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H22" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I22" s="1">
-        <v>0.26546999999999998</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1794,25 +1766,25 @@
         <v>402</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E23" s="1">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H23" s="1">
-        <v>5.9729999999999998E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I23" s="1">
-        <v>2.0299999999999998</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -1821,25 +1793,25 @@
         <v>402</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E24" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H24" s="1">
-        <v>0.13272999999999999</v>
+        <v>1.7219999999999999E-2</v>
       </c>
       <c r="I24" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.25829999999999997</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1848,25 +1820,25 @@
         <v>402</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H25" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.19869000000000001</v>
       </c>
       <c r="I25" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.99346000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
@@ -1875,10 +1847,10 @@
         <v>402</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -1887,13 +1859,13 @@
         <v>12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H26" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I26" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -1902,25 +1874,25 @@
         <v>402</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E27" s="1">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H27" s="1">
-        <v>1.7260000000000001E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I27" s="1">
-        <v>0.25883</v>
+        <v>0.26491999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -1929,25 +1901,25 @@
         <v>402</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E28" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H28" s="1">
-        <v>0.1991</v>
+        <v>5.9610000000000003E-2</v>
       </c>
       <c r="I28" s="1">
-        <v>0.99551000000000001</v>
+        <v>0.59606999999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
@@ -1956,13 +1928,13 @@
         <v>402</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D29" s="1" t="s">
         <v>88</v>
       </c>
+      <c r="D29" s="1">
+        <v>330</v>
+      </c>
       <c r="E29" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>12</v>
@@ -1971,10 +1943,10 @@
         <v>89</v>
       </c>
       <c r="H29" s="1">
-        <v>0.13272999999999999</v>
+        <v>2.9139999999999999E-2</v>
       </c>
       <c r="I29" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.29141</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
@@ -1989,7 +1961,7 @@
         <v>91</v>
       </c>
       <c r="E30" s="1">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>12</v>
@@ -1998,10 +1970,10 @@
         <v>92</v>
       </c>
       <c r="H30" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.42520000000000002</v>
       </c>
       <c r="I30" s="1">
-        <v>0.26546999999999998</v>
+        <v>7.23</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2016,7 +1988,7 @@
         <v>94</v>
       </c>
       <c r="E31" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>12</v>
@@ -2025,10 +1997,10 @@
         <v>95</v>
       </c>
       <c r="H31" s="1">
-        <v>5.9729999999999998E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I31" s="1">
-        <v>0.59731000000000001</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
@@ -2039,23 +2011,23 @@
       <c r="C32" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="D32" s="1">
-        <v>330</v>
+      <c r="D32" s="1" t="s">
+        <v>97</v>
       </c>
       <c r="E32" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H32" s="1">
-        <v>2.92E-2</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I32" s="1">
-        <v>0.29202</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2064,25 +2036,25 @@
         <v>402</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E33" s="1">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H33" s="1">
-        <v>0.42608000000000001</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I33" s="1">
-        <v>7.24</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
@@ -2091,10 +2063,10 @@
         <v>402</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E34" s="1">
         <v>1</v>
@@ -2103,13 +2075,13 @@
         <v>12</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H34" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I34" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2118,10 +2090,10 @@
         <v>402</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D35" s="1" t="s">
         <v>105</v>
+      </c>
+      <c r="D35" s="1">
+        <v>2</v>
       </c>
       <c r="E35" s="1">
         <v>1</v>
@@ -2133,10 +2105,10 @@
         <v>106</v>
       </c>
       <c r="H35" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I35" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
@@ -2160,16 +2132,16 @@
         <v>109</v>
       </c>
       <c r="H36" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I36" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>110</v>
@@ -2178,7 +2150,7 @@
         <v>111</v>
       </c>
       <c r="E37" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>12</v>
@@ -2187,22 +2159,22 @@
         <v>112</v>
       </c>
       <c r="H37" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.14438000000000001</v>
       </c>
       <c r="I37" s="1">
-        <v>0.13272999999999999</v>
+        <v>1.44</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D38" s="1">
-        <v>2</v>
+      <c r="D38" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="E38" s="1">
         <v>1</v>
@@ -2211,40 +2183,40 @@
         <v>12</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H38" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I38" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="1">
-        <v>402</v>
+        <v>603</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E39" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H39" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.35764000000000001</v>
       </c>
       <c r="I39" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.71528999999999998</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
@@ -2253,25 +2225,25 @@
         <v>603</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="E40" s="1">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="H40" s="1">
-        <v>0.14468</v>
+        <v>0.19869000000000001</v>
       </c>
       <c r="I40" s="1">
-        <v>1.45</v>
+        <v>0.19869000000000001</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
@@ -2280,25 +2252,25 @@
         <v>603</v>
       </c>
       <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="1">
-        <v>1</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="H41" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.29141</v>
       </c>
       <c r="I41" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.29141</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
@@ -2307,25 +2279,25 @@
         <v>603</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="E42" s="1">
+        <v>6</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E42" s="1">
-        <v>2</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="H42" s="1">
-        <v>0.35837999999999998</v>
+        <v>0.82125999999999999</v>
       </c>
       <c r="I42" s="1">
-        <v>0.71677000000000002</v>
+        <v>4.93</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
@@ -2334,11 +2306,11 @@
         <v>603</v>
       </c>
       <c r="C43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="E43" s="1">
         <v>1</v>
       </c>
@@ -2346,13 +2318,13 @@
         <v>12</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="H43" s="1">
-        <v>0.1991</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I43" s="1">
-        <v>0.1991</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
@@ -2361,10 +2333,10 @@
         <v>603</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E44" s="1">
         <v>1</v>
@@ -2373,73 +2345,73 @@
         <v>12</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H44" s="1">
-        <v>0.29202</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I44" s="1">
-        <v>0.29202</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="1">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E45" s="1">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H45" s="1">
-        <v>0.82296000000000002</v>
+        <v>0.50883</v>
       </c>
       <c r="I45" s="1">
-        <v>4.9400000000000004</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="1">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E46" s="1">
-        <v>1</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="H46" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.73692999999999997</v>
       </c>
       <c r="I46" s="1">
-        <v>0.13272999999999999</v>
+        <v>1.47</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="1">
-        <v>603</v>
+        <v>805</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>137</v>
@@ -2448,7 +2420,7 @@
         <v>138</v>
       </c>
       <c r="E47" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F47" s="1" t="s">
         <v>12</v>
@@ -2457,10 +2429,10 @@
         <v>139</v>
       </c>
       <c r="H47" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.42387999999999998</v>
       </c>
       <c r="I47" s="1">
-        <v>0.13272999999999999</v>
+        <v>0.84775</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
@@ -2475,7 +2447,7 @@
         <v>141</v>
       </c>
       <c r="E48" s="1">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>12</v>
@@ -2484,10 +2456,10 @@
         <v>142</v>
       </c>
       <c r="H48" s="1">
-        <v>0.51093999999999995</v>
+        <v>0.83450000000000002</v>
       </c>
       <c r="I48" s="1">
-        <v>5.1100000000000003</v>
+        <v>1.67</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
@@ -2502,19 +2474,19 @@
         <v>144</v>
       </c>
       <c r="E49" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H49" s="1">
-        <v>0.73997999999999997</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I49" s="1">
-        <v>1.48</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -2523,10 +2495,10 @@
         <v>805</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E50" s="1">
         <v>2</v>
@@ -2535,13 +2507,13 @@
         <v>12</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H50" s="1">
-        <v>0.42475000000000002</v>
+        <v>0.86099999999999999</v>
       </c>
       <c r="I50" s="1">
-        <v>0.84950000000000003</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -2550,25 +2522,25 @@
         <v>805</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E51" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H51" s="1">
-        <v>0.83623000000000003</v>
+        <v>0.13245999999999999</v>
       </c>
       <c r="I51" s="1">
-        <v>1.67</v>
+        <v>0.13245999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -2577,64 +2549,64 @@
         <v>805</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E52" s="1">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H52" s="1">
-        <v>0.55749000000000004</v>
+        <v>1.03</v>
       </c>
       <c r="I52" s="1">
-        <v>0.55749000000000004</v>
+        <v>8.27</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1"/>
       <c r="B53" s="1">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E53" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H53" s="1">
-        <v>0.13272999999999999</v>
+        <v>1.28</v>
       </c>
       <c r="I53" s="1">
-        <v>0.13272999999999999</v>
+        <v>2.57</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
       <c r="B54" s="1">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E54" s="1">
         <v>2</v>
@@ -2643,80 +2615,78 @@
         <v>12</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H54" s="1">
-        <v>0.86277999999999999</v>
+        <v>1.59</v>
       </c>
       <c r="I54" s="1">
-        <v>1.73</v>
+        <v>3.18</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1"/>
       <c r="B55" s="1">
-        <v>805</v>
+        <v>1206</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E55" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H55" s="1">
-        <v>0.13272999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="I55" s="1">
-        <v>0.13272999999999999</v>
+        <v>6.83</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1"/>
       <c r="B56" s="1">
-        <v>805</v>
+        <v>2220</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E56" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H56" s="1">
-        <v>1.04</v>
+        <v>3.42</v>
       </c>
       <c r="I56" s="1">
-        <v>8.2799999999999994</v>
+        <v>10.25</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1"/>
-      <c r="B57" s="1">
-        <v>1206</v>
+      <c r="B57" s="1" t="s">
+        <v>167</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>166</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="D57" s="1"/>
       <c r="E57" s="1">
         <v>2</v>
       </c>
@@ -2724,26 +2694,24 @@
         <v>12</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H57" s="1">
-        <v>1.29</v>
+        <v>1.81</v>
       </c>
       <c r="I57" s="1">
-        <v>2.58</v>
+        <v>3.63</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1"/>
-      <c r="B58" s="1">
-        <v>1206</v>
+      <c r="B58" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>169</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="D58" s="1"/>
       <c r="E58" s="1">
         <v>2</v>
       </c>
@@ -2751,76 +2719,72 @@
         <v>12</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H58" s="1">
-        <v>1.59</v>
+        <v>12.16</v>
       </c>
       <c r="I58" s="1">
-        <v>3.19</v>
+        <v>24.32</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1"/>
-      <c r="B59" s="1">
-        <v>1206</v>
+      <c r="B59" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>172</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="D59" s="1"/>
       <c r="E59" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H59" s="1">
-        <v>1.1399999999999999</v>
+        <v>7.11</v>
       </c>
       <c r="I59" s="1">
-        <v>6.85</v>
+        <v>7.11</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="1">
-        <v>2220</v>
+      <c r="B60" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>177</v>
+      </c>
+      <c r="D60" s="1"/>
       <c r="E60" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H60" s="1">
-        <v>3.42</v>
+        <v>0.56957999999999998</v>
       </c>
       <c r="I60" s="1">
-        <v>10.27</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1">
@@ -2830,22 +2794,22 @@
         <v>12</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H61" s="1">
-        <v>1.82</v>
+        <v>1.31</v>
       </c>
       <c r="I61" s="1">
-        <v>3.64</v>
+        <v>2.62</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1">
@@ -2855,22 +2819,22 @@
         <v>12</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H62" s="1">
-        <v>12.19</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="I62" s="1">
-        <v>24.37</v>
+        <v>4.4800000000000004</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1"/>
       <c r="B63" s="1" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1">
@@ -2880,197 +2844,197 @@
         <v>12</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H63" s="1">
-        <v>7.13</v>
+        <v>1.6</v>
       </c>
       <c r="I63" s="1">
-        <v>7.13</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
       <c r="B64" s="1" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="H64" s="1">
-        <v>0.57076000000000005</v>
+        <v>3.66</v>
       </c>
       <c r="I64" s="1">
-        <v>5.14</v>
+        <v>7.31</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1"/>
       <c r="B65" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H65" s="1">
-        <v>1.31</v>
+        <v>16.37</v>
       </c>
       <c r="I65" s="1">
-        <v>2.63</v>
+        <v>16.37</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
       <c r="B66" s="1" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H66" s="1">
-        <v>2.2400000000000002</v>
+        <v>1.92</v>
       </c>
       <c r="I66" s="1">
-        <v>4.49</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1"/>
       <c r="B67" s="1" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H67" s="1">
-        <v>1.61</v>
+        <v>2.27</v>
       </c>
       <c r="I67" s="1">
-        <v>1.61</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1"/>
       <c r="B68" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H68" s="1">
-        <v>3.66</v>
+        <v>0.40350999999999998</v>
       </c>
       <c r="I68" s="1">
-        <v>7.33</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H69" s="1">
-        <v>16.41</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="I69" s="1">
-        <v>16.41</v>
+        <v>4.13</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H70" s="1">
-        <v>1.92</v>
+        <v>0.40533000000000002</v>
       </c>
       <c r="I70" s="1">
-        <v>1.92</v>
+        <v>4.05</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1">
@@ -3080,122 +3044,122 @@
         <v>12</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="H71" s="1">
-        <v>2.27</v>
+        <v>3.97</v>
       </c>
       <c r="I71" s="1">
-        <v>4.54</v>
+        <v>7.95</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1"/>
       <c r="B72" s="1" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H72" s="1">
-        <v>0.40350999999999998</v>
+        <v>5.34</v>
       </c>
       <c r="I72" s="1">
-        <v>5.25</v>
+        <v>5.34</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="1" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H73" s="1">
-        <v>2.0699999999999998</v>
+        <v>1.02</v>
       </c>
       <c r="I73" s="1">
-        <v>4.1399999999999997</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H74" s="1">
-        <v>0.40616999999999998</v>
+        <v>3.02</v>
       </c>
       <c r="I74" s="1">
-        <v>4.0599999999999996</v>
+        <v>3.02</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1"/>
       <c r="B75" s="1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="H75" s="1">
-        <v>3.98</v>
+        <v>4.1500000000000004</v>
       </c>
       <c r="I75" s="1">
-        <v>7.96</v>
+        <v>4.1500000000000004</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1"/>
       <c r="B76" s="1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1">
@@ -3205,22 +3169,22 @@
         <v>12</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H76" s="1">
-        <v>5.35</v>
+        <v>0.88749</v>
       </c>
       <c r="I76" s="1">
-        <v>5.35</v>
+        <v>0.88749</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1"/>
       <c r="B77" s="1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1">
@@ -3230,245 +3194,145 @@
         <v>12</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H77" s="1">
-        <v>1.02</v>
+        <v>0.67554999999999998</v>
       </c>
       <c r="I77" s="1">
-        <v>1.02</v>
+        <v>0.67554999999999998</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1"/>
       <c r="B78" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H78" s="1">
-        <v>3.03</v>
+        <v>5.85</v>
       </c>
       <c r="I78" s="1">
-        <v>3.03</v>
+        <v>11.71</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1">
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="H79" s="1">
-        <v>4.1500000000000004</v>
+        <v>0.59606999999999999</v>
       </c>
       <c r="I79" s="1">
-        <v>4.1500000000000004</v>
+        <v>0.59606999999999999</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1"/>
       <c r="B80" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1">
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="H80" s="1">
-        <v>0.88932</v>
+        <v>28.9</v>
       </c>
       <c r="I80" s="1">
-        <v>0.88932</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1"/>
       <c r="B81" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H81" s="1">
-        <v>0.67695000000000005</v>
+        <v>1.62</v>
       </c>
       <c r="I81" s="1">
-        <v>0.67695000000000005</v>
+        <v>1.62</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1"/>
       <c r="B82" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D82" s="1"/>
+        <v>244</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="E82" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>12</v>
+        <v>235</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="H82" s="1">
-        <v>5.87</v>
+        <v>2.81</v>
       </c>
       <c r="I82" s="1">
-        <v>11.73</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1">
-        <v>1</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="H83" s="1">
-        <v>0.59731000000000001</v>
-      </c>
-      <c r="I83" s="1">
-        <v>0.59731000000000001</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1">
-        <v>1</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>249</v>
-      </c>
-      <c r="H84" s="1">
-        <v>28.96</v>
-      </c>
-      <c r="I84" s="1">
-        <v>28.96</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1">
-        <v>1</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="H85" s="1">
-        <v>1.62</v>
-      </c>
-      <c r="I85" s="1">
-        <v>1.62</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E86" s="1">
-        <v>1</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="H86" s="1">
-        <v>2.81</v>
-      </c>
-      <c r="I86" s="1">
         <v>2.81</v>
       </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="39" orientation="landscape" blackAndWhite="1" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="41" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>